<commit_message>
manual teszt elso 5db
</commit_message>
<xml_diff>
--- a/docs/Bug és manuál report.xlsx
+++ b/docs/Bug és manuál report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bisku\OneDrive\Dokumentumok\GitHub\MeetWave\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F24B77-56F2-4674-926C-CF74CB8DD131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F154E0AB-5AB4-47C5-8EAD-94DC7E6FC5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{262E611C-B263-43F7-AAE9-35116BAB0C88}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>MW-B-001</t>
   </si>
@@ -141,6 +141,66 @@
   </si>
   <si>
     <t>MW-B-014</t>
+  </si>
+  <si>
+    <t>MW-B-015</t>
+  </si>
+  <si>
+    <t>ha bejelentkezés gombra rákattint és nincs kitölve azt összes adat akkor a várt eredmény</t>
+  </si>
+  <si>
+    <t>1. Oldal betöltése 2. Regisztráció megnyitása 3. Adatok kitöltése</t>
+  </si>
+  <si>
+    <t>email: bármixy@gmail.com jelszó: barmixy jelszó még egyszer és telefonszám: 0630 325 2065</t>
+  </si>
+  <si>
+    <t>1. Oldal betöltése 2. Bejelentkezés megnyitása 3. Adatok kitöltése</t>
+  </si>
+  <si>
+    <t>Bejelentkezéskor a hiányzó adatnál a gombra rákattintva felugrik,hogy hiányzó adatok</t>
+  </si>
+  <si>
+    <t>Hiányzó adatnál sikeresen feldobja, hogy nem tud tovább menni hiányzó adat miatt</t>
+  </si>
+  <si>
+    <t>ha regisztráció gombra rákattint és nincs kitölve azt összes adat akkor a várt eredmény</t>
+  </si>
+  <si>
+    <t>Regisztárciókor a hiányzó adatnál a gombra rákattintva felugrik,hogy hiányzó adatok</t>
+  </si>
+  <si>
+    <t>lassú betöltési idő</t>
+  </si>
+  <si>
+    <t>nem reszponzív elrendezés</t>
+  </si>
+  <si>
+    <t>MeetWave logó nincs a helyén az eventnél</t>
+  </si>
+  <si>
+    <t>hiányzó popup animáció</t>
+  </si>
+  <si>
+    <t>keresési funkció helytelenségei</t>
+  </si>
+  <si>
+    <t>gyorsan betölt az oldal</t>
+  </si>
+  <si>
+    <t>nem tölt be az oldal (kb 1 perc)</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>oldal megnyitása event fül</t>
+  </si>
+  <si>
+    <t>nem reszponzív az event fül</t>
+  </si>
+  <si>
+    <t>reszponzív az event fül</t>
   </si>
 </sst>
 </file>
@@ -205,11 +265,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,8 +313,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>15356</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>910706</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>6559</xdr:rowOff>
     </xdr:to>
@@ -300,8 +357,8 @@
       <xdr:rowOff>24301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -344,8 +401,8 @@
       <xdr:rowOff>16221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6917</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438717</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -388,8 +445,8 @@
       <xdr:rowOff>2217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>935486</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>421136</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>6351</xdr:rowOff>
     </xdr:to>
@@ -432,8 +489,8 @@
       <xdr:rowOff>180685</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -476,8 +533,8 @@
       <xdr:rowOff>1035</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>431801</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -520,8 +577,8 @@
       <xdr:rowOff>176867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
@@ -564,8 +621,8 @@
       <xdr:rowOff>722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
       <xdr:row>123</xdr:row>
       <xdr:rowOff>16497</xdr:rowOff>
     </xdr:to>
@@ -608,8 +665,8 @@
       <xdr:rowOff>4307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>171663</xdr:rowOff>
     </xdr:to>
@@ -652,8 +709,8 @@
       <xdr:rowOff>9542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>882650</xdr:colOff>
       <xdr:row>148</xdr:row>
       <xdr:rowOff>178013</xdr:rowOff>
     </xdr:to>
@@ -696,8 +753,8 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>882650</xdr:colOff>
       <xdr:row>162</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -740,8 +797,8 @@
       <xdr:rowOff>8105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6351</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
       <xdr:row>175</xdr:row>
       <xdr:rowOff>6351</xdr:rowOff>
     </xdr:to>
@@ -784,8 +841,8 @@
       <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
       <xdr:row>188</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -828,8 +885,8 @@
       <xdr:rowOff>7643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>933451</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>882651</xdr:colOff>
       <xdr:row>201</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
@@ -1166,1202 +1223,1342 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752854D-7371-468D-9AE4-2CBC0C48C968}">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="J205" sqref="J205"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:13" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>45296.456250000003</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+    <row r="3" spans="1:13" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="3">
+        <v>45296.457638888889</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="3">
+        <v>45296.459027777775</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="101" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45296.461805555555</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45297.40902777778</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="7"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="7"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B72" s="7"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="7"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B85" s="7"/>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="7"/>
-      <c r="B88" s="7"/>
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="7"/>
-      <c r="B89" s="7"/>
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="7"/>
-      <c r="B90" s="7"/>
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="7"/>
-      <c r="B91" s="7"/>
+      <c r="A91" s="6"/>
+      <c r="B91" s="6"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
+      <c r="A92" s="6"/>
+      <c r="B92" s="6"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7"/>
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7"/>
+      <c r="A94" s="6"/>
+      <c r="B94" s="6"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7"/>
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="8"/>
-      <c r="B97" s="8"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B98" s="7"/>
+      <c r="B98" s="6"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7"/>
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7"/>
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7"/>
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
+      <c r="A107" s="6"/>
+      <c r="B107" s="6"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
+      <c r="A108" s="6"/>
+      <c r="B108" s="6"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
+      <c r="A109" s="6"/>
+      <c r="B109" s="6"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B111" s="7"/>
+      <c r="B111" s="6"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="7"/>
-      <c r="B112" s="7"/>
+      <c r="A112" s="6"/>
+      <c r="B112" s="6"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
+      <c r="A113" s="6"/>
+      <c r="B113" s="6"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="7"/>
-      <c r="B114" s="7"/>
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="7"/>
-      <c r="B115" s="7"/>
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="7"/>
-      <c r="B116" s="7"/>
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="7"/>
-      <c r="B117" s="7"/>
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="7"/>
-      <c r="B118" s="7"/>
+      <c r="A118" s="6"/>
+      <c r="B118" s="6"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="7"/>
-      <c r="B119" s="7"/>
+      <c r="A119" s="6"/>
+      <c r="B119" s="6"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="7"/>
-      <c r="B120" s="7"/>
+      <c r="A120" s="6"/>
+      <c r="B120" s="6"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="7"/>
-      <c r="B121" s="7"/>
+      <c r="A121" s="6"/>
+      <c r="B121" s="6"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="7"/>
-      <c r="B122" s="7"/>
+      <c r="A122" s="6"/>
+      <c r="B122" s="6"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="7" t="s">
+      <c r="A124" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B124" s="7"/>
+      <c r="B124" s="6"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="7"/>
-      <c r="B125" s="7"/>
+      <c r="A125" s="6"/>
+      <c r="B125" s="6"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="7"/>
-      <c r="B126" s="7"/>
+      <c r="A126" s="6"/>
+      <c r="B126" s="6"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="7"/>
-      <c r="B127" s="7"/>
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="7"/>
-      <c r="B128" s="7"/>
+      <c r="A128" s="6"/>
+      <c r="B128" s="6"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="7"/>
-      <c r="B129" s="7"/>
+      <c r="A129" s="6"/>
+      <c r="B129" s="6"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="7"/>
-      <c r="B130" s="7"/>
+      <c r="A130" s="6"/>
+      <c r="B130" s="6"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="7"/>
-      <c r="B131" s="7"/>
+      <c r="A131" s="6"/>
+      <c r="B131" s="6"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="7"/>
-      <c r="B132" s="7"/>
+      <c r="A132" s="6"/>
+      <c r="B132" s="6"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="7"/>
-      <c r="B133" s="7"/>
+      <c r="A133" s="6"/>
+      <c r="B133" s="6"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="7"/>
-      <c r="B134" s="7"/>
+      <c r="A134" s="6"/>
+      <c r="B134" s="6"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="7"/>
-      <c r="B135" s="7"/>
+      <c r="A135" s="6"/>
+      <c r="B135" s="6"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="8"/>
-      <c r="B136" s="8"/>
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="7" t="s">
+      <c r="A137" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B137" s="7"/>
+      <c r="B137" s="6"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="7"/>
-      <c r="B138" s="7"/>
+      <c r="A138" s="6"/>
+      <c r="B138" s="6"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="7"/>
-      <c r="B141" s="7"/>
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
+      <c r="A142" s="6"/>
+      <c r="B142" s="6"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
+      <c r="A143" s="6"/>
+      <c r="B143" s="6"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="7"/>
-      <c r="B145" s="7"/>
+      <c r="A145" s="6"/>
+      <c r="B145" s="6"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
+      <c r="A146" s="6"/>
+      <c r="B146" s="6"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="7"/>
-      <c r="B147" s="7"/>
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
+      <c r="A149" s="7"/>
+      <c r="B149" s="7"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B150" s="7"/>
+      <c r="B150" s="6"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
+      <c r="A157" s="6"/>
+      <c r="B157" s="6"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="8"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="7"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="7" t="s">
+      <c r="A163" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B163" s="7"/>
+      <c r="B163" s="6"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" s="7"/>
-      <c r="B169" s="7"/>
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" s="7"/>
-      <c r="B171" s="7"/>
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="7"/>
-      <c r="B173" s="7"/>
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="8"/>
-      <c r="B175" s="8"/>
+      <c r="A175" s="7"/>
+      <c r="B175" s="7"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="7" t="s">
+      <c r="A176" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B176" s="7"/>
+      <c r="B176" s="6"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" s="7"/>
-      <c r="B179" s="7"/>
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" s="7"/>
-      <c r="B180" s="7"/>
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="7"/>
-      <c r="B181" s="7"/>
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" s="7"/>
-      <c r="B182" s="7"/>
+      <c r="A182" s="6"/>
+      <c r="B182" s="6"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="7"/>
-      <c r="B183" s="7"/>
+      <c r="A183" s="6"/>
+      <c r="B183" s="6"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" s="7"/>
-      <c r="B184" s="7"/>
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="7"/>
-      <c r="B185" s="7"/>
+      <c r="A185" s="6"/>
+      <c r="B185" s="6"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" s="7"/>
-      <c r="B186" s="7"/>
+      <c r="A186" s="6"/>
+      <c r="B186" s="6"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="7"/>
-      <c r="B187" s="7"/>
+      <c r="A187" s="6"/>
+      <c r="B187" s="6"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="8"/>
-      <c r="B188" s="8"/>
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="7" t="s">
+      <c r="A189" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B189" s="7"/>
+      <c r="B189" s="6"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="7"/>
-      <c r="B190" s="7"/>
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="7"/>
-      <c r="B191" s="7"/>
+      <c r="A191" s="6"/>
+      <c r="B191" s="6"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" s="7"/>
-      <c r="B192" s="7"/>
+      <c r="A192" s="6"/>
+      <c r="B192" s="6"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="7"/>
-      <c r="B193" s="7"/>
+      <c r="A193" s="6"/>
+      <c r="B193" s="6"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" s="7"/>
-      <c r="B194" s="7"/>
+      <c r="A194" s="6"/>
+      <c r="B194" s="6"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A195" s="7"/>
-      <c r="B195" s="7"/>
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" s="7"/>
-      <c r="B196" s="7"/>
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" s="7"/>
-      <c r="B197" s="7"/>
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" s="7"/>
-      <c r="B198" s="7"/>
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" s="7"/>
-      <c r="B199" s="7"/>
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" s="7"/>
-      <c r="B200" s="7"/>
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" s="8"/>
-      <c r="B201" s="8"/>
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A20:B32"/>
+    <mergeCell ref="A33:B45"/>
+    <mergeCell ref="A46:B58"/>
+    <mergeCell ref="A59:B71"/>
+    <mergeCell ref="A72:B84"/>
     <mergeCell ref="A150:B162"/>
     <mergeCell ref="A163:B175"/>
     <mergeCell ref="A176:B188"/>
@@ -2371,11 +2568,6 @@
     <mergeCell ref="A111:B123"/>
     <mergeCell ref="A124:B136"/>
     <mergeCell ref="A137:B149"/>
-    <mergeCell ref="A20:B32"/>
-    <mergeCell ref="A33:B45"/>
-    <mergeCell ref="A46:B58"/>
-    <mergeCell ref="A59:B71"/>
-    <mergeCell ref="A72:B84"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>